<commit_message>
Clean export Excel. Old version removed, unused files removed
</commit_message>
<xml_diff>
--- a/IJC_UI/Template.xlsx
+++ b/IJC_UI/Template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\git\IJC_UI\IJC_UI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Pion" sheetId="3" r:id="rId1"/>
@@ -25,12 +30,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Pion!$B$3:$J$53</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Toren!$B$3:$J$57</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t>Groep</t>
   </si>
@@ -80,16 +85,13 @@
     <t>Periode X, Ronde X</t>
   </si>
   <si>
-    <t>Kloktijd 2x30 min. Trio 2x20 min.</t>
-  </si>
-  <si>
     <t>KONINGSGROEP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -306,6 +308,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -353,7 +358,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -386,9 +391,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -421,6 +443,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -1427,7 +1466,7 @@
   <dimension ref="A3:K62"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,7 +1484,7 @@
     <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="16"/>
@@ -4722,7 +4761,7 @@
   </sheetPr>
   <dimension ref="A3:K62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -4741,7 +4780,7 @@
     <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="16"/>
@@ -4757,7 +4796,7 @@
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="str">
         <f>VLOOKUP(C3,Data!A2:B8,2,FALSE)</f>
-        <v>Kloktijd 2x30 min. Trio 2x20 min.</v>
+        <v>Kloktijd 2x60 min. Trio 2x40 min.</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -5546,7 +5585,7 @@
   </sheetPr>
   <dimension ref="A3:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -6368,7 +6407,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6395,10 +6434,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added API support for Plone CMS 5.2
Export Uitslag en Stand naar Plone CMS 5.2
</commit_message>
<xml_diff>
--- a/IJC_UI/Template.xlsx
+++ b/IJC_UI/Template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\git\IJC_UI\IJC_UI\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Pion" sheetId="3" r:id="rId1"/>
@@ -30,12 +25,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Pion!$B$3:$J$53</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Toren!$B$3:$J$57</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
   <si>
     <t>Groep</t>
   </si>
@@ -85,13 +80,16 @@
     <t>Periode X, Ronde X</t>
   </si>
   <si>
+    <t>Kloktijd 2x30 min. Trio 2x20 min.</t>
+  </si>
+  <si>
     <t>KONINGSGROEP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -308,9 +306,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -358,7 +353,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -391,26 +386,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,23 +421,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -1466,7 +1427,7 @@
   <dimension ref="A3:K62"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,7 +1445,7 @@
     <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="16"/>
@@ -4761,7 +4722,7 @@
   </sheetPr>
   <dimension ref="A3:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -4780,7 +4741,7 @@
     <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="16"/>
@@ -4796,7 +4757,7 @@
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="str">
         <f>VLOOKUP(C3,Data!A2:B8,2,FALSE)</f>
-        <v>Kloktijd 2x60 min. Trio 2x40 min.</v>
+        <v>Kloktijd 2x30 min. Trio 2x20 min.</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -5585,7 +5546,7 @@
   </sheetPr>
   <dimension ref="A3:K62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -6407,7 +6368,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6434,10 +6395,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>